<commit_message>
version101: add nextcloud sharing stuff
</commit_message>
<xml_diff>
--- a/SValimaki.xlsx
+++ b/SValimaki.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:H3"/>
+  <dimension ref="A2:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,62 @@
         <v>0.7177188976041666</v>
       </c>
     </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>43423</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0.4584691899189815</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>43423</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0.4818042578125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>43423</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>0.4890109440046296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>43423</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0.4937088486111111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
remove spaces from sheet names
</commit_message>
<xml_diff>
--- a/SValimaki.xlsx
+++ b/SValimaki.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="SValimaki                                       " sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="SValimaki" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
@@ -519,4 +520,37 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>43423</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0.5084813385416667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>